<commit_message>
fixed tailing correction display added laboratory numbers to PrBlank.xlsx, Ratios.xlsx and Ratios_add.xlsx
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/PrBlank.xlsx
+++ b/data/CPR_100221_20210210-114741/PrBlank.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+  <si>
+    <t>Lab. #</t>
+  </si>
   <si>
     <t>U-233</t>
   </si>
@@ -53,12 +56,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,23 +379,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -410,290 +421,326 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1">
+      <c r="A2" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B2" s="1">
         <v>3.901846046034124E-06</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1">
         <v>17.22533069182192</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="1">
         <v>1.14469468685095E-05</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="1">
         <v>1.384573122361481E-05</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="1">
         <v>0.0008982322321794075</v>
       </c>
-      <c r="F2">
+      <c r="G2" s="1">
         <v>5.526572353886759</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="1">
         <v>1.740829020128608E-05</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="1">
         <v>4.655388565839045</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3">
+        <v>10989</v>
+      </c>
+      <c r="B3">
         <v>1.316099150030235E-05</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>12.74495436747084</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>4.752379390516241E-06</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.0009824356551704626</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2.705596032409401</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3.658636756655603E-06</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3.908659429673211</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
+    <row r="4" spans="1:9" s="1" customFormat="1">
+      <c r="A4" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="1">
         <v>11.00258612354965</v>
       </c>
-      <c r="C4">
+      <c r="D4" s="1">
         <v>1.95740077564445E-05</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="1">
         <v>2.660938286452046E-06</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="1">
         <v>0.002688347267077272</v>
       </c>
-      <c r="F4">
+      <c r="G4" s="1">
         <v>3.908659448070066</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="1">
         <v>1.705030403570207E-06</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="1">
         <v>11.5004057249031</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5">
+        <v>10990</v>
+      </c>
+      <c r="B5">
         <v>5.215417591584224E-06</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>9.633582632866894</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2.703996910681676E-07</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.001159727398048135</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3.473067515571064</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>8.437930452719581E-06</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>6.688150948162487</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
+    <row r="6" spans="1:9" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B6" s="1">
         <v>9.439146870734528E-06</v>
       </c>
-      <c r="B6">
+      <c r="C6" s="1">
         <v>16.7275108483419</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="1">
         <v>1.241681767155806E-05</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="1">
         <v>2.365672157128165E-05</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="1">
         <v>0.002971992056955079</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="1">
         <v>6.771120831476206</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="1">
         <v>3.795088587079014E-06</v>
       </c>
-      <c r="H6">
+      <c r="I6" s="1">
         <v>10.50476661319143</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7">
+        <v>10991</v>
+      </c>
+      <c r="B7">
         <v>1.046778088837101E-05</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>7.849729581210092</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>3.844421408746303E-06</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.969918815070323E-06</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.001451388430518423</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4.945783136666423</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>7.393395098558572</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8">
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B8" s="1">
         <v>4.22826976915021E-06</v>
       </c>
-      <c r="B8">
+      <c r="C8" s="1">
         <v>16.10523644160163</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="1">
         <v>1.515938105860515E-05</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="1">
         <v>1.693250859983226E-05</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="1">
         <v>0.003960029546390261</v>
       </c>
-      <c r="F8">
+      <c r="G8" s="1">
         <v>2.913020753353904</v>
       </c>
-      <c r="G8">
+      <c r="H8" s="1">
         <v>7.786401248113158E-06</v>
       </c>
-      <c r="H8">
+      <c r="I8" s="1">
         <v>4.655388508868135</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9">
+        <v>10992</v>
+      </c>
+      <c r="B9">
         <v>3.386070518327416E-06</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>6.190331562032536</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1.843959140640061E-05</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.00163468700728592</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2.601883677278171</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>6.118590747548409E-06</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>3.410840106053008</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
+    <row r="10" spans="1:9" s="1" customFormat="1">
+      <c r="A10" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B10" s="1">
         <v>1.361934218274018E-05</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="1">
         <v>15.10959716055964</v>
       </c>
-      <c r="C10">
+      <c r="D10" s="1">
         <v>1.635066095006342E-05</v>
       </c>
-      <c r="D10">
+      <c r="E10" s="1">
         <v>1.367569800035122E-06</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="1">
         <v>0.004017310985721586</v>
       </c>
-      <c r="F10">
+      <c r="G10" s="1">
         <v>2.041836938996706</v>
       </c>
-      <c r="G10">
+      <c r="H10" s="1">
         <v>1.420902319000492E-06</v>
       </c>
-      <c r="H10">
+      <c r="I10" s="1">
         <v>6.356271337363864</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11">
+        <v>10993</v>
+      </c>
+      <c r="B11">
         <v>2.49477190203762E-06</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>5.19469282142314</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2.204685145534101E-05</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.809886463003301E-05</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>0.001870717256853382</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1.232880578863894</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>8.823552247720535E-06</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2.705596049025914</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1">
+        <v>10815</v>
+      </c>
+      <c r="B12" s="1">
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="1">
         <v>12.8694093770035</v>
       </c>
-      <c r="C12">
+      <c r="D12" s="1">
         <v>2.384616369396851E-05</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="F12" s="1">
         <v>0.003497545038600171</v>
       </c>
-      <c r="F12">
+      <c r="G12" s="1">
         <v>1.792927305672054</v>
       </c>
-      <c r="G12">
+      <c r="H12" s="1">
         <v>1.079019353511607E-05</v>
       </c>
-      <c r="H12">
+      <c r="I12" s="1">
         <v>5.028752984373324</v>
       </c>
     </row>

</xml_diff>

<commit_message>
output folder feature - extra context can be saved - repeated analyses are saved seperately
</commit_message>
<xml_diff>
--- a/data/CPR_100221_20210210-114741/PrBlank.xlsx
+++ b/data/CPR_100221_20210210-114741/PrBlank.xlsx
@@ -47,13 +47,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -82,9 +88,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,32 +465,32 @@
         <v>4.655388565839045</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
+    <row r="3" spans="1:9" s="2" customFormat="1">
+      <c r="A3" s="2">
         <v>10989</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>1.316099150030235E-05</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>12.74495436747084</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>4.752379390516241E-06</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.0009824356551704626</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>2.705596032409401</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>3.658636756655603E-06</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>3.908659429673211</v>
       </c>
     </row>
@@ -512,32 +523,32 @@
         <v>11.5004057249031</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
+    <row r="5" spans="1:9" s="2" customFormat="1">
+      <c r="A5" s="2">
         <v>10990</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>5.215417591584224E-06</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>9.633582632866894</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>2.703996910681676E-07</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.001159727398048135</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>3.473067515571064</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>8.437930452719581E-06</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>6.688150948162487</v>
       </c>
     </row>
@@ -570,32 +581,32 @@
         <v>10.50476661319143</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
+    <row r="7" spans="1:9" s="2" customFormat="1">
+      <c r="A7" s="2">
         <v>10991</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1.046778088837101E-05</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>7.849729581210092</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>3.844421408746303E-06</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1.969918815070323E-06</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.001451388430518423</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>4.945783136666423</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>7.393395098558572</v>
       </c>
     </row>
@@ -628,32 +639,32 @@
         <v>4.655388508868135</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
+    <row r="9" spans="1:9" s="2" customFormat="1">
+      <c r="A9" s="2">
         <v>10992</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>3.386070518327416E-06</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>6.190331562032536</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>1.843959140640061E-05</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0.00163468700728592</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>2.601883677278171</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>6.118590747548409E-06</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>3.410840106053008</v>
       </c>
     </row>
@@ -686,32 +697,32 @@
         <v>6.356271337363864</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
+    <row r="11" spans="1:9" s="2" customFormat="1">
+      <c r="A11" s="2">
         <v>10993</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>2.49477190203762E-06</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>5.19469282142314</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>2.204685145534101E-05</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1.809886463003301E-05</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.001870717256853382</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>1.232880578863894</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>8.823552247720535E-06</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>2.705596049025914</v>
       </c>
     </row>

</xml_diff>